<commit_message>
Initial commit of WhatsApp salary slip sender
</commit_message>
<xml_diff>
--- a/salary_template.xlsx
+++ b/salary_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\53\systems\Finance\WhatsaApp_sys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F46567D-BC8F-40D2-BBD8-9D30642CAA38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932C7A2C-1E1B-411B-B74A-171423CEFB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{A6E5440B-EB67-4483-BD6D-3A637333E02E}"/>
+    <workbookView xWindow="-38520" yWindow="-1935" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{A6E5440B-EB67-4483-BD6D-3A637333E02E}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -185,7 +185,7 @@
     <t>mmnnbk</t>
   </si>
   <si>
-    <t>اللواء 53 مشاة مستقل القسم المالي</t>
+    <t>اللواء 53 مشاة مسقل القسم المالي</t>
   </si>
 </sst>
 </file>
@@ -1847,8 +1847,8 @@
   <sheetPr codeName="data1"/>
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView rightToLeft="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2160,7 +2160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFFF21-CA5D-4C13-92EC-176FD3572423}">
   <dimension ref="B2:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" rightToLeft="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" rightToLeft="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="P10" sqref="P10:Q10"/>
     </sheetView>
   </sheetViews>

</xml_diff>